<commit_message>
Excel data reader & Data driven approach
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -123,10 +123,10 @@
     <t xml:space="preserve">Would like to provide selenium training for beginners</t>
   </si>
   <si>
-    <t xml:space="preserve">Programming &amp; Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA</t>
+    <t xml:space="preserve">Digital Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Marketing</t>
   </si>
   <si>
     <t xml:space="preserve">Testing</t>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">On-site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12042022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12052022</t>
   </si>
   <si>
     <t xml:space="preserve">Mon</t>
@@ -151,12 +157,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -192,6 +199,14 @@
       <color rgb="FF008000"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,7 +260,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,11 +277,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,7 +357,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFA31515"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -354,7 +377,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -418,11 +441,11 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -488,15 +511,15 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
@@ -556,17 +579,17 @@
       </c>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -578,32 +601,32 @@
       <c r="G2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>43567</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>43597</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="I2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>29</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>